<commit_message>
add multi-sheet reading for excel sheets (#202)
* add multi-sheet reading for excel sheets

* fix typo

* bump minor version
</commit_message>
<xml_diff>
--- a/spreadsheet_conversion/single_subject_sheet/subject_metadata_multisheet_example.xlsx
+++ b/spreadsheet_conversion/single_subject_sheet/subject_metadata_multisheet_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galassiae/Projects/PET2BIDS/spreadsheet_conversion/single_subject_sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2D8015-BF3F-414C-9000-B5F7A9B3660D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C8094F-3E5E-A742-A1D9-4D89C2166351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>

</xml_diff>